<commit_message>
Add Query to Read Suppliers Data and Display in DataGridView
</commit_message>
<xml_diff>
--- a/Oxygen supplier.xlsx
+++ b/Oxygen supplier.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0135BB2-7033-47EA-840B-D210F0202C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" xr2:uid="{7919A9C7-DAD9-493E-AD43-A51699F5B9F8}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +23,34 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,13 +395,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5199EEEB-4138-4EB2-B704-64EF5DE6CDB7}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row spans="1:7" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>TestUser</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>123411313612</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>blaabla</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="inlineStr">
+        <is>
+          <t>TestComapny</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>